<commit_message>
PID rates (not tested but compiling)
</commit_message>
<xml_diff>
--- a/execute/10.2.2.xlsx
+++ b/execute/10.2.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spencer\repos\courses\advanced_flight_sim\execute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE12F0C-9CD8-4398-B711-481B6FF7B51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B25135-85AD-4AE0-9293-81EC675AC9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{1D1C15E7-0565-4DAC-B796-9DDB6424A202}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{1D1C15E7-0565-4DAC-B796-9DDB6424A202}"/>
   </bookViews>
   <sheets>
     <sheet name="time_const=0.05" sheetId="1" r:id="rId1"/>
@@ -5675,8 +5675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD33CE5-A3E7-4A3D-A3A9-4B5A545B8401}">
   <dimension ref="A1:V202"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19427,8 +19427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D90FF68-CC3D-4DDD-AB4D-C458CE131B0E}">
   <dimension ref="A1:V202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>